<commit_message>
Updated unittests for GetQuarterCoordinates
</commit_message>
<xml_diff>
--- a/unittests calculations.xlsx
+++ b/unittests calculations.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LHS calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="scheme 2 LHS calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="Quarter coordinates calculation" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>nr</t>
   </si>
@@ -69,6 +70,36 @@
   </si>
   <si>
     <t>N_O2</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>r0</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>x_offset</t>
+  </si>
+  <si>
+    <t>y_offset</t>
+  </si>
+  <si>
+    <t>x_dist</t>
+  </si>
+  <si>
+    <t>y_dist</t>
+  </si>
+  <si>
+    <t>coordinates</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>rounded</t>
   </si>
 </sst>
 </file>
@@ -388,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="Q62" sqref="Q62"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1226,7 @@
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="F15:O15" si="2">H3</f>
+        <f t="shared" ref="H15:O15" si="2">H3</f>
         <v>3</v>
       </c>
       <c r="I15">
@@ -1276,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" ref="F16:O16" si="4">I4</f>
+        <f t="shared" ref="I16:O16" si="4">I4</f>
         <v>4</v>
       </c>
       <c r="J16">
@@ -1355,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="J17">
-        <f t="shared" ref="F17:O17" si="6">J5</f>
+        <f t="shared" ref="J17:O17" si="6">J5</f>
         <v>5</v>
       </c>
       <c r="K17">
@@ -1432,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <f t="shared" ref="F18:O18" si="8">K6</f>
+        <f t="shared" ref="K18:O18" si="8">K6</f>
         <v>6</v>
       </c>
       <c r="L18">
@@ -1507,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <f t="shared" ref="F19:O19" si="10">L7</f>
+        <f t="shared" ref="L19:O19" si="10">L7</f>
         <v>7</v>
       </c>
       <c r="M19">
@@ -1580,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="F20:O20" si="12">M8</f>
+        <f t="shared" ref="M20:O20" si="12">M8</f>
         <v>8</v>
       </c>
       <c r="N20">
@@ -1651,7 +1682,7 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <f t="shared" ref="F21:O21" si="14">N9</f>
+        <f t="shared" ref="N21:O21" si="14">N9</f>
         <v>9</v>
       </c>
       <c r="O21">
@@ -1720,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="F22:O22" si="16">O10</f>
+        <f t="shared" ref="O22" si="16">O10</f>
         <v>10</v>
       </c>
       <c r="Q22">
@@ -1894,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <f t="shared" ref="F27:O27" si="18">G3</f>
+        <f t="shared" ref="G27" si="18">G3</f>
         <v>-2</v>
       </c>
       <c r="H27">
@@ -1925,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="R27">
-        <f t="shared" ref="R27:Z27" si="19">R3</f>
+        <f t="shared" ref="R27" si="19">R3</f>
         <v>-2</v>
       </c>
       <c r="S27">
@@ -1961,7 +1992,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="F28:O28" si="20">H4</f>
+        <f t="shared" ref="H28" si="20">H4</f>
         <v>-2</v>
       </c>
       <c r="I28">
@@ -1992,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="S28">
-        <f t="shared" ref="S28:Z28" si="21">S4</f>
+        <f t="shared" ref="S28" si="21">S4</f>
         <v>-2</v>
       </c>
       <c r="T28">
@@ -2028,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" ref="F29:O29" si="22">I5</f>
+        <f t="shared" ref="I29" si="22">I5</f>
         <v>-2</v>
       </c>
       <c r="J29">
@@ -2059,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <f t="shared" ref="T29:Z29" si="23">T5</f>
+        <f t="shared" ref="T29" si="23">T5</f>
         <v>-2</v>
       </c>
       <c r="U29">
@@ -2095,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="J30">
-        <f t="shared" ref="F30:O30" si="24">J6</f>
+        <f t="shared" ref="J30" si="24">J6</f>
         <v>-2</v>
       </c>
       <c r="K30">
@@ -2126,7 +2157,7 @@
         <v>0</v>
       </c>
       <c r="U30">
-        <f t="shared" ref="U30:Z30" si="25">U6</f>
+        <f t="shared" ref="U30" si="25">U6</f>
         <v>-2</v>
       </c>
       <c r="V30">
@@ -2162,7 +2193,7 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="F31:O31" si="26">K7</f>
+        <f t="shared" ref="K31" si="26">K7</f>
         <v>-2</v>
       </c>
       <c r="L31">
@@ -2193,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="V31">
-        <f t="shared" ref="V31:Z31" si="27">V7</f>
+        <f t="shared" ref="V31" si="27">V7</f>
         <v>-2</v>
       </c>
       <c r="W31">
@@ -2229,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="F32:O32" si="28">L8</f>
+        <f t="shared" ref="L32" si="28">L8</f>
         <v>-2</v>
       </c>
       <c r="M32">
@@ -2260,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" ref="W32:Z32" si="29">W8</f>
+        <f t="shared" ref="W32" si="29">W8</f>
         <v>-2</v>
       </c>
       <c r="X32">
@@ -2296,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" ref="F33:O33" si="30">M9</f>
+        <f t="shared" ref="M33" si="30">M9</f>
         <v>-2</v>
       </c>
       <c r="N33">
@@ -2327,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="X33">
-        <f t="shared" ref="X33:Z33" si="31">X9</f>
+        <f t="shared" ref="X33" si="31">X9</f>
         <v>-2</v>
       </c>
       <c r="Y33">
@@ -2363,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <f t="shared" ref="F34:O34" si="32">N10</f>
+        <f t="shared" ref="N34" si="32">N10</f>
         <v>-2</v>
       </c>
       <c r="O34">
@@ -2394,7 +2425,7 @@
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="shared" ref="Y34:Z34" si="33">Y10</f>
+        <f t="shared" ref="Y34" si="33">Y10</f>
         <v>-2</v>
       </c>
       <c r="Z34">
@@ -2430,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" ref="F35:O35" si="34">O11</f>
+        <f t="shared" ref="O35" si="34">O11</f>
         <v>3</v>
       </c>
       <c r="Q35">
@@ -2537,7 +2568,7 @@
     </row>
     <row r="39" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F39">
-        <f t="shared" ref="F39:O39" si="36">F3</f>
+        <f t="shared" ref="F39" si="36">F3</f>
         <v>-1</v>
       </c>
       <c r="G39">
@@ -2568,7 +2599,7 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" ref="Q39:Z39" si="37">Q3</f>
+        <f t="shared" ref="Q39" si="37">Q3</f>
         <v>-1</v>
       </c>
       <c r="R39">
@@ -2601,7 +2632,7 @@
     </row>
     <row r="40" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F40">
-        <f t="shared" ref="F40:O40" si="38">F4</f>
+        <f t="shared" ref="F40:G40" si="38">F4</f>
         <v>0</v>
       </c>
       <c r="G40">
@@ -2633,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" ref="Q40:Z40" si="39">Q4</f>
+        <f t="shared" ref="Q40:R40" si="39">Q4</f>
         <v>0</v>
       </c>
       <c r="R40">
@@ -2667,7 +2698,7 @@
     </row>
     <row r="41" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F41">
-        <f t="shared" ref="F41:O41" si="40">F5</f>
+        <f t="shared" ref="F41:H41" si="40">F5</f>
         <v>0</v>
       </c>
       <c r="G41">
@@ -2700,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" ref="Q41:Z41" si="41">Q5</f>
+        <f t="shared" ref="Q41:S41" si="41">Q5</f>
         <v>0</v>
       </c>
       <c r="R41">
@@ -2735,7 +2766,7 @@
     </row>
     <row r="42" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F42">
-        <f t="shared" ref="F42:O42" si="42">F6</f>
+        <f t="shared" ref="F42:I42" si="42">F6</f>
         <v>0</v>
       </c>
       <c r="G42">
@@ -2769,7 +2800,7 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" ref="Q42:Z42" si="43">Q6</f>
+        <f t="shared" ref="Q42:T42" si="43">Q6</f>
         <v>0</v>
       </c>
       <c r="R42">
@@ -2805,7 +2836,7 @@
     </row>
     <row r="43" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F43">
-        <f t="shared" ref="F43:O43" si="44">F7</f>
+        <f t="shared" ref="F43:J43" si="44">F7</f>
         <v>0</v>
       </c>
       <c r="G43">
@@ -2840,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" ref="Q43:Z43" si="45">Q7</f>
+        <f t="shared" ref="Q43:U43" si="45">Q7</f>
         <v>0</v>
       </c>
       <c r="R43">
@@ -2877,7 +2908,7 @@
     </row>
     <row r="44" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F44">
-        <f t="shared" ref="F44:O44" si="46">F8</f>
+        <f t="shared" ref="F44:K44" si="46">F8</f>
         <v>0</v>
       </c>
       <c r="G44">
@@ -2913,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" ref="Q44:Z44" si="47">Q8</f>
+        <f t="shared" ref="Q44:V44" si="47">Q8</f>
         <v>0</v>
       </c>
       <c r="R44">
@@ -2951,7 +2982,7 @@
     </row>
     <row r="45" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F45">
-        <f t="shared" ref="F45:O45" si="48">F9</f>
+        <f t="shared" ref="F45:L45" si="48">F9</f>
         <v>0</v>
       </c>
       <c r="G45">
@@ -2988,7 +3019,7 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="shared" ref="Q45:Z45" si="49">Q9</f>
+        <f t="shared" ref="Q45:W45" si="49">Q9</f>
         <v>0</v>
       </c>
       <c r="R45">
@@ -3027,7 +3058,7 @@
     </row>
     <row r="46" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F46">
-        <f t="shared" ref="F46:O46" si="50">F10</f>
+        <f t="shared" ref="F46:M46" si="50">F10</f>
         <v>0</v>
       </c>
       <c r="G46">
@@ -3065,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <f t="shared" ref="Q46:Z46" si="51">Q10</f>
+        <f t="shared" ref="Q46:X46" si="51">Q10</f>
         <v>0</v>
       </c>
       <c r="R46">
@@ -3105,7 +3136,7 @@
     </row>
     <row r="47" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F47">
-        <f t="shared" ref="F47:O47" si="52">F11</f>
+        <f t="shared" ref="F47:N47" si="52">F11</f>
         <v>0</v>
       </c>
       <c r="G47">
@@ -3144,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" ref="Q47:Z47" si="53">Q11</f>
+        <f t="shared" ref="Q47:Y47" si="53">Q11</f>
         <v>0</v>
       </c>
       <c r="R47">
@@ -3193,821 +3224,821 @@
     </row>
     <row r="50" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F50">
-        <f>1/$B$2*F26+F38</f>
+        <f t="shared" ref="F50:O50" si="54">1/$B$2*F26+F38</f>
         <v>-2</v>
       </c>
       <c r="G50">
-        <f>1/$B$2*G26+G38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="H50">
-        <f>1/$B$2*H26+H38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="I50">
-        <f>1/$B$2*I26+I38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="J50">
-        <f>1/$B$2*J26+J38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="K50">
-        <f>1/$B$2*K26+K38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="L50">
-        <f>1/$B$2*L26+L38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="M50">
-        <f>1/$B$2*M26+M38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="N50">
-        <f>1/$B$2*N26+N38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="O50">
-        <f>1/$B$2*O26+O38</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="Q50">
-        <f>1/$B$2*Q26+Q38</f>
+        <f t="shared" ref="Q50:Z50" si="55">1/$B$2*Q26+Q38</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="R50">
-        <f>1/$B$2*R26+R38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="S50">
-        <f>1/$B$2*S26+S38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="T50">
-        <f>1/$B$2*T26+T38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="U50">
-        <f>1/$B$2*U26+U38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="V50">
-        <f>1/$B$2*V26+V38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="W50">
-        <f>1/$B$2*W26+W38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="X50">
-        <f>1/$B$2*X26+X38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Y50">
-        <f>1/$B$2*Y26+Y38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="Z50">
-        <f>1/$B$2*Z26+Z38</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F51">
-        <f>1/$B$2*F27+F39</f>
+        <f t="shared" ref="F51:O51" si="56">1/$B$2*F27+F39</f>
         <v>-1</v>
       </c>
       <c r="G51">
-        <f>1/$B$2*G27+G39</f>
+        <f t="shared" si="56"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="H51">
-        <f>1/$B$2*H27+H39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="I51">
-        <f>1/$B$2*I27+I39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="J51">
-        <f>1/$B$2*J27+J39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="K51">
-        <f>1/$B$2*K27+K39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="L51">
-        <f>1/$B$2*L27+L39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="M51">
-        <f>1/$B$2*M27+M39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="N51">
-        <f>1/$B$2*N27+N39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="O51">
-        <f>1/$B$2*O27+O39</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="Q51">
-        <f>1/$B$2*Q27+Q39</f>
+        <f t="shared" ref="Q51:Z51" si="57">1/$B$2*Q27+Q39</f>
         <v>-1</v>
       </c>
       <c r="R51">
-        <f>1/$B$2*R27+R39</f>
+        <f t="shared" si="57"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="S51">
-        <f>1/$B$2*S27+S39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="T51">
-        <f>1/$B$2*T27+T39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="U51">
-        <f>1/$B$2*U27+U39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="V51">
-        <f>1/$B$2*V27+V39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="W51">
-        <f>1/$B$2*W27+W39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="X51">
-        <f>1/$B$2*X27+X39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="Y51">
-        <f>1/$B$2*Y27+Y39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="Z51">
-        <f>1/$B$2*Z27+Z39</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F52">
-        <f>1/$B$2*F28+F40</f>
+        <f t="shared" ref="F52:O52" si="58">1/$B$2*F28+F40</f>
         <v>0</v>
       </c>
       <c r="G52">
-        <f>1/$B$2*G28+G40</f>
+        <f t="shared" si="58"/>
         <v>-2</v>
       </c>
       <c r="H52">
-        <f>1/$B$2*H28+H40</f>
+        <f t="shared" si="58"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="I52">
-        <f>1/$B$2*I28+I40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="J52">
-        <f>1/$B$2*J28+J40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="K52">
-        <f>1/$B$2*K28+K40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="L52">
-        <f>1/$B$2*L28+L40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="M52">
-        <f>1/$B$2*M28+M40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="N52">
-        <f>1/$B$2*N28+N40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="O52">
-        <f>1/$B$2*O28+O40</f>
+        <f t="shared" si="58"/>
         <v>0</v>
       </c>
       <c r="Q52">
-        <f>1/$B$2*Q28+Q40</f>
+        <f t="shared" ref="Q52:Z52" si="59">1/$B$2*Q28+Q40</f>
         <v>0</v>
       </c>
       <c r="R52">
-        <f>1/$B$2*R28+R40</f>
+        <f t="shared" si="59"/>
         <v>-2</v>
       </c>
       <c r="S52">
-        <f>1/$B$2*S28+S40</f>
+        <f t="shared" si="59"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="T52">
-        <f>1/$B$2*T28+T40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="U52">
-        <f>1/$B$2*U28+U40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="V52">
-        <f>1/$B$2*V28+V40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="W52">
-        <f>1/$B$2*W28+W40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="X52">
-        <f>1/$B$2*X28+X40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="Y52">
-        <f>1/$B$2*Y28+Y40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
       <c r="Z52">
-        <f>1/$B$2*Z28+Z40</f>
+        <f t="shared" si="59"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F53">
-        <f>1/$B$2*F29+F41</f>
+        <f t="shared" ref="F53:O53" si="60">1/$B$2*F29+F41</f>
         <v>0</v>
       </c>
       <c r="G53">
-        <f>1/$B$2*G29+G41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="H53">
-        <f>1/$B$2*H29+H41</f>
+        <f t="shared" si="60"/>
         <v>-3</v>
       </c>
       <c r="I53">
-        <f>1/$B$2*I29+I41</f>
+        <f t="shared" si="60"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="J53">
-        <f>1/$B$2*J29+J41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="K53">
-        <f>1/$B$2*K29+K41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="L53">
-        <f>1/$B$2*L29+L41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="M53">
-        <f>1/$B$2*M29+M41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="N53">
-        <f>1/$B$2*N29+N41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="O53">
-        <f>1/$B$2*O29+O41</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="Q53">
-        <f>1/$B$2*Q29+Q41</f>
+        <f t="shared" ref="Q53:Z53" si="61">1/$B$2*Q29+Q41</f>
         <v>0</v>
       </c>
       <c r="R53">
-        <f>1/$B$2*R29+R41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="S53">
-        <f>1/$B$2*S29+S41</f>
+        <f t="shared" si="61"/>
         <v>-3</v>
       </c>
       <c r="T53">
-        <f>1/$B$2*T29+T41</f>
+        <f t="shared" si="61"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="U53">
-        <f>1/$B$2*U29+U41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="V53">
-        <f>1/$B$2*V29+V41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="W53">
-        <f>1/$B$2*W29+W41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="X53">
-        <f>1/$B$2*X29+X41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="Y53">
-        <f>1/$B$2*Y29+Y41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
       <c r="Z53">
-        <f>1/$B$2*Z29+Z41</f>
+        <f t="shared" si="61"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F54">
-        <f>1/$B$2*F30+F42</f>
+        <f t="shared" ref="F54:O54" si="62">1/$B$2*F30+F42</f>
         <v>0</v>
       </c>
       <c r="G54">
-        <f>1/$B$2*G30+G42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="H54">
-        <f>1/$B$2*H30+H42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="I54">
-        <f>1/$B$2*I30+I42</f>
+        <f t="shared" si="62"/>
         <v>-4</v>
       </c>
       <c r="J54">
-        <f>1/$B$2*J30+J42</f>
+        <f t="shared" si="62"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="K54">
-        <f>1/$B$2*K30+K42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="L54">
-        <f>1/$B$2*L30+L42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="M54">
-        <f>1/$B$2*M30+M42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="N54">
-        <f>1/$B$2*N30+N42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O54">
-        <f>1/$B$2*O30+O42</f>
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="Q54">
-        <f>1/$B$2*Q30+Q42</f>
+        <f t="shared" ref="Q54:Z54" si="63">1/$B$2*Q30+Q42</f>
         <v>0</v>
       </c>
       <c r="R54">
-        <f>1/$B$2*R30+R42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="S54">
-        <f>1/$B$2*S30+S42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="T54">
-        <f>1/$B$2*T30+T42</f>
+        <f t="shared" si="63"/>
         <v>-4</v>
       </c>
       <c r="U54">
-        <f>1/$B$2*U30+U42</f>
+        <f t="shared" si="63"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="V54">
-        <f>1/$B$2*V30+V42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="W54">
-        <f>1/$B$2*W30+W42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="X54">
-        <f>1/$B$2*X30+X42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Y54">
-        <f>1/$B$2*Y30+Y42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
       <c r="Z54">
-        <f>1/$B$2*Z30+Z42</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F55">
-        <f>1/$B$2*F31+F43</f>
+        <f t="shared" ref="F55:O55" si="64">1/$B$2*F31+F43</f>
         <v>0</v>
       </c>
       <c r="G55">
-        <f>1/$B$2*G31+G43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="H55">
-        <f>1/$B$2*H31+H43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="I55">
-        <f>1/$B$2*I31+I43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="J55">
-        <f>1/$B$2*J31+J43</f>
+        <f t="shared" si="64"/>
         <v>-5</v>
       </c>
       <c r="K55">
-        <f>1/$B$2*K31+K43</f>
+        <f t="shared" si="64"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="L55">
-        <f>1/$B$2*L31+L43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="M55">
-        <f>1/$B$2*M31+M43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="N55">
-        <f>1/$B$2*N31+N43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="O55">
-        <f>1/$B$2*O31+O43</f>
+        <f t="shared" si="64"/>
         <v>0</v>
       </c>
       <c r="Q55">
-        <f>1/$B$2*Q31+Q43</f>
+        <f t="shared" ref="Q55:Z55" si="65">1/$B$2*Q31+Q43</f>
         <v>0</v>
       </c>
       <c r="R55">
-        <f>1/$B$2*R31+R43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="S55">
-        <f>1/$B$2*S31+S43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="T55">
-        <f>1/$B$2*T31+T43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="U55">
-        <f>1/$B$2*U31+U43</f>
+        <f t="shared" si="65"/>
         <v>-5</v>
       </c>
       <c r="V55">
-        <f>1/$B$2*V31+V43</f>
+        <f t="shared" si="65"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="W55">
-        <f>1/$B$2*W31+W43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="X55">
-        <f>1/$B$2*X31+X43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="Y55">
-        <f>1/$B$2*Y31+Y43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
       <c r="Z55">
-        <f>1/$B$2*Z31+Z43</f>
+        <f t="shared" si="65"/>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F56">
-        <f>1/$B$2*F32+F44</f>
+        <f t="shared" ref="F56:O56" si="66">1/$B$2*F32+F44</f>
         <v>0</v>
       </c>
       <c r="G56">
-        <f>1/$B$2*G32+G44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="H56">
-        <f>1/$B$2*H32+H44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="I56">
-        <f>1/$B$2*I32+I44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="J56">
-        <f>1/$B$2*J32+J44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="K56">
-        <f>1/$B$2*K32+K44</f>
+        <f t="shared" si="66"/>
         <v>-6</v>
       </c>
       <c r="L56">
-        <f>1/$B$2*L32+L44</f>
+        <f t="shared" si="66"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="M56">
-        <f>1/$B$2*M32+M44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="N56">
-        <f>1/$B$2*N32+N44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="O56">
-        <f>1/$B$2*O32+O44</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="Q56">
-        <f>1/$B$2*Q32+Q44</f>
+        <f t="shared" ref="Q56:Z56" si="67">1/$B$2*Q32+Q44</f>
         <v>0</v>
       </c>
       <c r="R56">
-        <f>1/$B$2*R32+R44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="S56">
-        <f>1/$B$2*S32+S44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="T56">
-        <f>1/$B$2*T32+T44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="U56">
-        <f>1/$B$2*U32+U44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="V56">
-        <f>1/$B$2*V32+V44</f>
+        <f t="shared" si="67"/>
         <v>-6</v>
       </c>
       <c r="W56">
-        <f>1/$B$2*W32+W44</f>
+        <f t="shared" si="67"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="X56">
-        <f>1/$B$2*X32+X44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="Y56">
-        <f>1/$B$2*Y32+Y44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="Z56">
-        <f>1/$B$2*Z32+Z44</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F57">
-        <f>1/$B$2*F33+F45</f>
+        <f t="shared" ref="F57:O57" si="68">1/$B$2*F33+F45</f>
         <v>0</v>
       </c>
       <c r="G57">
-        <f>1/$B$2*G33+G45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="H57">
-        <f>1/$B$2*H33+H45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="I57">
-        <f>1/$B$2*I33+I45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="J57">
-        <f>1/$B$2*J33+J45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="K57">
-        <f>1/$B$2*K33+K45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="L57">
-        <f>1/$B$2*L33+L45</f>
+        <f t="shared" si="68"/>
         <v>-7</v>
       </c>
       <c r="M57">
-        <f>1/$B$2*M33+M45</f>
+        <f t="shared" si="68"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="N57">
-        <f>1/$B$2*N33+N45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="O57">
-        <f>1/$B$2*O33+O45</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="Q57">
-        <f>1/$B$2*Q33+Q45</f>
+        <f t="shared" ref="Q57:Z57" si="69">1/$B$2*Q33+Q45</f>
         <v>0</v>
       </c>
       <c r="R57">
-        <f>1/$B$2*R33+R45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="S57">
-        <f>1/$B$2*S33+S45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="T57">
-        <f>1/$B$2*T33+T45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="U57">
-        <f>1/$B$2*U33+U45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="V57">
-        <f>1/$B$2*V33+V45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="W57">
-        <f>1/$B$2*W33+W45</f>
+        <f t="shared" si="69"/>
         <v>-7</v>
       </c>
       <c r="X57">
-        <f>1/$B$2*X33+X45</f>
+        <f t="shared" si="69"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="Y57">
-        <f>1/$B$2*Y33+Y45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
       <c r="Z57">
-        <f>1/$B$2*Z33+Z45</f>
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F58">
-        <f>1/$B$2*F34+F46</f>
+        <f t="shared" ref="F58:O58" si="70">1/$B$2*F34+F46</f>
         <v>0</v>
       </c>
       <c r="G58">
-        <f>1/$B$2*G34+G46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="H58">
-        <f>1/$B$2*H34+H46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="I58">
-        <f>1/$B$2*I34+I46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="J58">
-        <f>1/$B$2*J34+J46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="K58">
-        <f>1/$B$2*K34+K46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="L58">
-        <f>1/$B$2*L34+L46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="M58">
-        <f>1/$B$2*M34+M46</f>
+        <f t="shared" si="70"/>
         <v>-8</v>
       </c>
       <c r="N58">
-        <f>1/$B$2*N34+N46</f>
+        <f t="shared" si="70"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="O58">
-        <f>1/$B$2*O34+O46</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="Q58">
-        <f>1/$B$2*Q34+Q46</f>
+        <f t="shared" ref="Q58:Z58" si="71">1/$B$2*Q34+Q46</f>
         <v>0</v>
       </c>
       <c r="R58">
-        <f>1/$B$2*R34+R46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="S58">
-        <f>1/$B$2*S34+S46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="T58">
-        <f>1/$B$2*T34+T46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="U58">
-        <f>1/$B$2*U34+U46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="V58">
-        <f>1/$B$2*V34+V46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="W58">
-        <f>1/$B$2*W34+W46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
       <c r="X58">
-        <f>1/$B$2*X34+X46</f>
+        <f t="shared" si="71"/>
         <v>-8</v>
       </c>
       <c r="Y58">
-        <f>1/$B$2*Y34+Y46</f>
+        <f t="shared" si="71"/>
         <v>-1.3333333333333333</v>
       </c>
       <c r="Z58">
-        <f>1/$B$2*Z34+Z46</f>
+        <f t="shared" si="71"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F59">
-        <f>1/$B$2*F35+F47</f>
+        <f t="shared" ref="F59:O59" si="72">1/$B$2*F35+F47</f>
         <v>0</v>
       </c>
       <c r="G59">
-        <f>1/$B$2*G35+G47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="H59">
-        <f>1/$B$2*H35+H47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="I59">
-        <f>1/$B$2*I35+I47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="J59">
-        <f>1/$B$2*J35+J47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="K59">
-        <f>1/$B$2*K35+K47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="L59">
-        <f>1/$B$2*L35+L47</f>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="M59">
-        <f>1/$B$2*M35+M47</f>
+        <f t="shared" si="72"/>
         <v>1</v>
       </c>
       <c r="N59">
-        <f>1/$B$2*N35+N47</f>
+        <f t="shared" si="72"/>
         <v>-4</v>
       </c>
       <c r="O59">
-        <f>1/$B$2*O35+O47</f>
+        <f t="shared" si="72"/>
         <v>2</v>
       </c>
       <c r="Q59">
-        <f>1/$B$2*Q35+Q47</f>
+        <f t="shared" ref="Q59:Z59" si="73">1/$B$2*Q35+Q47</f>
         <v>0</v>
       </c>
       <c r="R59">
-        <f>1/$B$2*R35+R47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="S59">
-        <f>1/$B$2*S35+S47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="T59">
-        <f>1/$B$2*T35+T47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="U59">
-        <f>1/$B$2*U35+U47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="V59">
-        <f>1/$B$2*V35+V47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="W59">
-        <f>1/$B$2*W35+W47</f>
+        <f t="shared" si="73"/>
         <v>0</v>
       </c>
       <c r="X59">
-        <f>1/$B$2*X35+X47</f>
+        <f t="shared" si="73"/>
         <v>1</v>
       </c>
       <c r="Y59">
-        <f>1/$B$2*Y35+Y47</f>
+        <f t="shared" si="73"/>
         <v>-4</v>
       </c>
       <c r="Z59">
-        <f>1/$B$2*Z35+Z47</f>
+        <f t="shared" si="73"/>
         <v>2</v>
       </c>
     </row>
@@ -4021,822 +4052,971 @@
     </row>
     <row r="62" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F62">
-        <f>(1/$B$2-1)*F26-F14</f>
+        <f t="shared" ref="F62:O62" si="74">(1/$B$2-1)*F26-F14</f>
         <v>1</v>
       </c>
       <c r="G62">
-        <f>(1/$B$2-1)*G26-G14</f>
+        <f t="shared" si="74"/>
         <v>-4</v>
       </c>
       <c r="H62">
-        <f>(1/$B$2-1)*H26-H14</f>
+        <f t="shared" si="74"/>
         <v>1</v>
       </c>
       <c r="I62">
-        <f>(1/$B$2-1)*I26-I14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="J62">
-        <f>(1/$B$2-1)*J26-J14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="K62">
-        <f>(1/$B$2-1)*K26-K14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="L62">
-        <f>(1/$B$2-1)*L26-L14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="M62">
-        <f>(1/$B$2-1)*M26-M14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="N62">
-        <f>(1/$B$2-1)*N26-N14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="O62">
-        <f>(1/$B$2-1)*O26-O14</f>
+        <f t="shared" si="74"/>
         <v>0</v>
       </c>
       <c r="Q62">
-        <f>(1/$B$2-1)*Q26-Q14</f>
+        <f t="shared" ref="Q62:Z62" si="75">(1/$B$2-1)*Q26-Q14</f>
         <v>-0.33333333333333337</v>
       </c>
       <c r="R62">
-        <f>(1/$B$2-1)*R26-R14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="S62">
-        <f>(1/$B$2-1)*S26-S14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="T62">
-        <f>(1/$B$2-1)*T26-T14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="U62">
-        <f>(1/$B$2-1)*U26-U14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="V62">
-        <f>(1/$B$2-1)*V26-V14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="W62">
-        <f>(1/$B$2-1)*W26-W14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="X62">
-        <f>(1/$B$2-1)*X26-X14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="Y62">
-        <f>(1/$B$2-1)*Y26-Y14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
       <c r="Z62">
-        <f>(1/$B$2-1)*Z26-Z14</f>
+        <f t="shared" si="75"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F63">
-        <f>(1/$B$2-1)*F27-F15</f>
+        <f t="shared" ref="F63:O63" si="76">(1/$B$2-1)*F27-F15</f>
         <v>0</v>
       </c>
       <c r="G63">
-        <f>(1/$B$2-1)*G27-G15</f>
+        <f t="shared" si="76"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="H63">
-        <f>(1/$B$2-1)*H27-H15</f>
+        <f t="shared" si="76"/>
         <v>-3</v>
       </c>
       <c r="I63">
-        <f>(1/$B$2-1)*I27-I15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="J63">
-        <f>(1/$B$2-1)*J27-J15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="K63">
-        <f>(1/$B$2-1)*K27-K15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="L63">
-        <f>(1/$B$2-1)*L27-L15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="M63">
-        <f>(1/$B$2-1)*M27-M15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="N63">
-        <f>(1/$B$2-1)*N27-N15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="O63">
-        <f>(1/$B$2-1)*O27-O15</f>
+        <f t="shared" si="76"/>
         <v>0</v>
       </c>
       <c r="Q63">
-        <f>(1/$B$2-1)*Q27-Q15</f>
+        <f t="shared" ref="Q63:Z63" si="77">(1/$B$2-1)*Q27-Q15</f>
         <v>0</v>
       </c>
       <c r="R63">
-        <f>(1/$B$2-1)*R27-R15</f>
+        <f t="shared" si="77"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="S63">
-        <f>(1/$B$2-1)*S27-S15</f>
+        <f t="shared" si="77"/>
         <v>-3</v>
       </c>
       <c r="T63">
-        <f>(1/$B$2-1)*T27-T15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="U63">
-        <f>(1/$B$2-1)*U27-U15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="V63">
-        <f>(1/$B$2-1)*V27-V15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="W63">
-        <f>(1/$B$2-1)*W27-W15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="X63">
-        <f>(1/$B$2-1)*X27-X15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="Y63">
-        <f>(1/$B$2-1)*Y27-Y15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
       <c r="Z63">
-        <f>(1/$B$2-1)*Z27-Z15</f>
+        <f t="shared" si="77"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F64">
-        <f>(1/$B$2-1)*F28-F16</f>
+        <f t="shared" ref="F64:O64" si="78">(1/$B$2-1)*F28-F16</f>
         <v>0</v>
       </c>
       <c r="G64">
-        <f>(1/$B$2-1)*G28-G16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="H64">
-        <f>(1/$B$2-1)*H28-H16</f>
+        <f t="shared" si="78"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="I64">
-        <f>(1/$B$2-1)*I28-I16</f>
+        <f t="shared" si="78"/>
         <v>-4</v>
       </c>
       <c r="J64">
-        <f>(1/$B$2-1)*J28-J16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="K64">
-        <f>(1/$B$2-1)*K28-K16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="L64">
-        <f>(1/$B$2-1)*L28-L16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="M64">
-        <f>(1/$B$2-1)*M28-M16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="N64">
-        <f>(1/$B$2-1)*N28-N16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="O64">
-        <f>(1/$B$2-1)*O28-O16</f>
+        <f t="shared" si="78"/>
         <v>0</v>
       </c>
       <c r="Q64">
-        <f>(1/$B$2-1)*Q28-Q16</f>
+        <f t="shared" ref="Q64:Z64" si="79">(1/$B$2-1)*Q28-Q16</f>
         <v>0</v>
       </c>
       <c r="R64">
-        <f>(1/$B$2-1)*R28-R16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="S64">
-        <f>(1/$B$2-1)*S28-S16</f>
+        <f t="shared" si="79"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="T64">
-        <f>(1/$B$2-1)*T28-T16</f>
+        <f t="shared" si="79"/>
         <v>-4</v>
       </c>
       <c r="U64">
-        <f>(1/$B$2-1)*U28-U16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="V64">
-        <f>(1/$B$2-1)*V28-V16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="W64">
-        <f>(1/$B$2-1)*W28-W16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="X64">
-        <f>(1/$B$2-1)*X28-X16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="Y64">
-        <f>(1/$B$2-1)*Y28-Y16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
       <c r="Z64">
-        <f>(1/$B$2-1)*Z28-Z16</f>
+        <f t="shared" si="79"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F65">
-        <f>(1/$B$2-1)*F29-F17</f>
+        <f t="shared" ref="F65:O65" si="80">(1/$B$2-1)*F29-F17</f>
         <v>0</v>
       </c>
       <c r="G65">
-        <f>(1/$B$2-1)*G29-G17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="H65">
-        <f>(1/$B$2-1)*H29-H17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="I65">
-        <f>(1/$B$2-1)*I29-I17</f>
+        <f t="shared" si="80"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="J65">
-        <f>(1/$B$2-1)*J29-J17</f>
+        <f t="shared" si="80"/>
         <v>-5</v>
       </c>
       <c r="K65">
-        <f>(1/$B$2-1)*K29-K17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="L65">
-        <f>(1/$B$2-1)*L29-L17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="M65">
-        <f>(1/$B$2-1)*M29-M17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="N65">
-        <f>(1/$B$2-1)*N29-N17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="O65">
-        <f>(1/$B$2-1)*O29-O17</f>
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
       <c r="Q65">
-        <f>(1/$B$2-1)*Q29-Q17</f>
+        <f t="shared" ref="Q65:Z65" si="81">(1/$B$2-1)*Q29-Q17</f>
         <v>0</v>
       </c>
       <c r="R65">
-        <f>(1/$B$2-1)*R29-R17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="S65">
-        <f>(1/$B$2-1)*S29-S17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="T65">
-        <f>(1/$B$2-1)*T29-T17</f>
+        <f t="shared" si="81"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="U65">
-        <f>(1/$B$2-1)*U29-U17</f>
+        <f t="shared" si="81"/>
         <v>-5</v>
       </c>
       <c r="V65">
-        <f>(1/$B$2-1)*V29-V17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="W65">
-        <f>(1/$B$2-1)*W29-W17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="X65">
-        <f>(1/$B$2-1)*X29-X17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="Y65">
-        <f>(1/$B$2-1)*Y29-Y17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
       <c r="Z65">
-        <f>(1/$B$2-1)*Z29-Z17</f>
+        <f t="shared" si="81"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F66">
-        <f>(1/$B$2-1)*F30-F18</f>
+        <f t="shared" ref="F66:O66" si="82">(1/$B$2-1)*F30-F18</f>
         <v>0</v>
       </c>
       <c r="G66">
-        <f>(1/$B$2-1)*G30-G18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="H66">
-        <f>(1/$B$2-1)*H30-H18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="I66">
-        <f>(1/$B$2-1)*I30-I18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="J66">
-        <f>(1/$B$2-1)*J30-J18</f>
+        <f t="shared" si="82"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K66">
-        <f>(1/$B$2-1)*K30-K18</f>
+        <f t="shared" si="82"/>
         <v>-6</v>
       </c>
       <c r="L66">
-        <f>(1/$B$2-1)*L30-L18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="M66">
-        <f>(1/$B$2-1)*M30-M18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="N66">
-        <f>(1/$B$2-1)*N30-N18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="O66">
-        <f>(1/$B$2-1)*O30-O18</f>
+        <f t="shared" si="82"/>
         <v>0</v>
       </c>
       <c r="Q66">
-        <f>(1/$B$2-1)*Q30-Q18</f>
+        <f t="shared" ref="Q66:Z66" si="83">(1/$B$2-1)*Q30-Q18</f>
         <v>0</v>
       </c>
       <c r="R66">
-        <f>(1/$B$2-1)*R30-R18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="S66">
-        <f>(1/$B$2-1)*S30-S18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="T66">
-        <f>(1/$B$2-1)*T30-T18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="U66">
-        <f>(1/$B$2-1)*U30-U18</f>
+        <f t="shared" si="83"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="V66">
-        <f>(1/$B$2-1)*V30-V18</f>
+        <f t="shared" si="83"/>
         <v>-6</v>
       </c>
       <c r="W66">
-        <f>(1/$B$2-1)*W30-W18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="X66">
-        <f>(1/$B$2-1)*X30-X18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="Y66">
-        <f>(1/$B$2-1)*Y30-Y18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
       <c r="Z66">
-        <f>(1/$B$2-1)*Z30-Z18</f>
+        <f t="shared" si="83"/>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F67">
-        <f>(1/$B$2-1)*F31-F19</f>
+        <f t="shared" ref="F67:O67" si="84">(1/$B$2-1)*F31-F19</f>
         <v>0</v>
       </c>
       <c r="G67">
-        <f>(1/$B$2-1)*G31-G19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="H67">
-        <f>(1/$B$2-1)*H31-H19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="I67">
-        <f>(1/$B$2-1)*I31-I19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="J67">
-        <f>(1/$B$2-1)*J31-J19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="K67">
-        <f>(1/$B$2-1)*K31-K19</f>
+        <f t="shared" si="84"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="L67">
-        <f>(1/$B$2-1)*L31-L19</f>
+        <f t="shared" si="84"/>
         <v>-7</v>
       </c>
       <c r="M67">
-        <f>(1/$B$2-1)*M31-M19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="N67">
-        <f>(1/$B$2-1)*N31-N19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="O67">
-        <f>(1/$B$2-1)*O31-O19</f>
+        <f t="shared" si="84"/>
         <v>0</v>
       </c>
       <c r="Q67">
-        <f>(1/$B$2-1)*Q31-Q19</f>
+        <f t="shared" ref="Q67:Z67" si="85">(1/$B$2-1)*Q31-Q19</f>
         <v>0</v>
       </c>
       <c r="R67">
-        <f>(1/$B$2-1)*R31-R19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="S67">
-        <f>(1/$B$2-1)*S31-S19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="T67">
-        <f>(1/$B$2-1)*T31-T19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="U67">
-        <f>(1/$B$2-1)*U31-U19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="V67">
-        <f>(1/$B$2-1)*V31-V19</f>
+        <f t="shared" si="85"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="W67">
-        <f>(1/$B$2-1)*W31-W19</f>
+        <f t="shared" si="85"/>
         <v>-7</v>
       </c>
       <c r="X67">
-        <f>(1/$B$2-1)*X31-X19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Y67">
-        <f>(1/$B$2-1)*Y31-Y19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
       <c r="Z67">
-        <f>(1/$B$2-1)*Z31-Z19</f>
+        <f t="shared" si="85"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F68">
-        <f>(1/$B$2-1)*F32-F20</f>
+        <f t="shared" ref="F68:O68" si="86">(1/$B$2-1)*F32-F20</f>
         <v>0</v>
       </c>
       <c r="G68">
-        <f>(1/$B$2-1)*G32-G20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="H68">
-        <f>(1/$B$2-1)*H32-H20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="I68">
-        <f>(1/$B$2-1)*I32-I20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="J68">
-        <f>(1/$B$2-1)*J32-J20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="K68">
-        <f>(1/$B$2-1)*K32-K20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="L68">
-        <f>(1/$B$2-1)*L32-L20</f>
+        <f t="shared" si="86"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="M68">
-        <f>(1/$B$2-1)*M32-M20</f>
+        <f t="shared" si="86"/>
         <v>-8</v>
       </c>
       <c r="N68">
-        <f>(1/$B$2-1)*N32-N20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="O68">
-        <f>(1/$B$2-1)*O32-O20</f>
+        <f t="shared" si="86"/>
         <v>0</v>
       </c>
       <c r="Q68">
-        <f>(1/$B$2-1)*Q32-Q20</f>
+        <f t="shared" ref="Q68:Z68" si="87">(1/$B$2-1)*Q32-Q20</f>
         <v>0</v>
       </c>
       <c r="R68">
-        <f>(1/$B$2-1)*R32-R20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="S68">
-        <f>(1/$B$2-1)*S32-S20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="T68">
-        <f>(1/$B$2-1)*T32-T20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="U68">
-        <f>(1/$B$2-1)*U32-U20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="V68">
-        <f>(1/$B$2-1)*V32-V20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="W68">
-        <f>(1/$B$2-1)*W32-W20</f>
+        <f t="shared" si="87"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="X68">
-        <f>(1/$B$2-1)*X32-X20</f>
+        <f t="shared" si="87"/>
         <v>-8</v>
       </c>
       <c r="Y68">
-        <f>(1/$B$2-1)*Y32-Y20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
       <c r="Z68">
-        <f>(1/$B$2-1)*Z32-Z20</f>
+        <f t="shared" si="87"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F69">
-        <f>(1/$B$2-1)*F33-F21</f>
+        <f t="shared" ref="F69:O69" si="88">(1/$B$2-1)*F33-F21</f>
         <v>0</v>
       </c>
       <c r="G69">
-        <f>(1/$B$2-1)*G33-G21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f>(1/$B$2-1)*H33-H21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="I69">
-        <f>(1/$B$2-1)*I33-I21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="J69">
-        <f>(1/$B$2-1)*J33-J21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="K69">
-        <f>(1/$B$2-1)*K33-K21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="L69">
-        <f>(1/$B$2-1)*L33-L21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="M69">
-        <f>(1/$B$2-1)*M33-M21</f>
+        <f t="shared" si="88"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="N69">
-        <f>(1/$B$2-1)*N33-N21</f>
+        <f t="shared" si="88"/>
         <v>-9</v>
       </c>
       <c r="O69">
-        <f>(1/$B$2-1)*O33-O21</f>
+        <f t="shared" si="88"/>
         <v>0</v>
       </c>
       <c r="Q69">
-        <f>(1/$B$2-1)*Q33-Q21</f>
+        <f t="shared" ref="Q69:Z69" si="89">(1/$B$2-1)*Q33-Q21</f>
         <v>0</v>
       </c>
       <c r="R69">
-        <f>(1/$B$2-1)*R33-R21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="S69">
-        <f>(1/$B$2-1)*S33-S21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="T69">
-        <f>(1/$B$2-1)*T33-T21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="U69">
-        <f>(1/$B$2-1)*U33-U21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="V69">
-        <f>(1/$B$2-1)*V33-V21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="W69">
-        <f>(1/$B$2-1)*W33-W21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
       <c r="X69">
-        <f>(1/$B$2-1)*X33-X21</f>
+        <f t="shared" si="89"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="Y69">
-        <f>(1/$B$2-1)*Y33-Y21</f>
+        <f t="shared" si="89"/>
         <v>-9</v>
       </c>
       <c r="Z69">
-        <f>(1/$B$2-1)*Z33-Z21</f>
+        <f t="shared" si="89"/>
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F70">
-        <f>(1/$B$2-1)*F34-F22</f>
+        <f t="shared" ref="F70:O70" si="90">(1/$B$2-1)*F34-F22</f>
         <v>0</v>
       </c>
       <c r="G70">
-        <f>(1/$B$2-1)*G34-G22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="H70">
-        <f>(1/$B$2-1)*H34-H22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="I70">
-        <f>(1/$B$2-1)*I34-I22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="J70">
-        <f>(1/$B$2-1)*J34-J22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="K70">
-        <f>(1/$B$2-1)*K34-K22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="L70">
-        <f>(1/$B$2-1)*L34-L22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="M70">
-        <f>(1/$B$2-1)*M34-M22</f>
+        <f t="shared" si="90"/>
         <v>0</v>
       </c>
       <c r="N70">
-        <f>(1/$B$2-1)*N34-N22</f>
+        <f t="shared" si="90"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="O70">
-        <f>(1/$B$2-1)*O34-O22</f>
+        <f t="shared" si="90"/>
         <v>-10</v>
       </c>
       <c r="Q70">
-        <f>(1/$B$2-1)*Q34-Q22</f>
+        <f t="shared" ref="Q70:Z70" si="91">(1/$B$2-1)*Q34-Q22</f>
         <v>0</v>
       </c>
       <c r="R70">
-        <f>(1/$B$2-1)*R34-R22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="S70">
-        <f>(1/$B$2-1)*S34-S22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="T70">
-        <f>(1/$B$2-1)*T34-T22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="U70">
-        <f>(1/$B$2-1)*U34-U22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="V70">
-        <f>(1/$B$2-1)*V34-V22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="W70">
-        <f>(1/$B$2-1)*W34-W22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="X70">
-        <f>(1/$B$2-1)*X34-X22</f>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="Y70">
-        <f>(1/$B$2-1)*Y34-Y22</f>
+        <f t="shared" si="91"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="Z70">
-        <f>(1/$B$2-1)*Z34-Z22</f>
+        <f t="shared" si="91"/>
         <v>-10</v>
       </c>
     </row>
     <row r="71" spans="6:26" x14ac:dyDescent="0.25">
       <c r="F71">
-        <f>(1/$B$2-1)*F35-F23</f>
+        <f t="shared" ref="F71:O71" si="92">(1/$B$2-1)*F35-F23</f>
         <v>0</v>
       </c>
       <c r="G71">
-        <f>(1/$B$2-1)*G35-G23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="H71">
-        <f>(1/$B$2-1)*H35-H23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="I71">
-        <f>(1/$B$2-1)*I35-I23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="J71">
-        <f>(1/$B$2-1)*J35-J23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="K71">
-        <f>(1/$B$2-1)*K35-K23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="L71">
-        <f>(1/$B$2-1)*L35-L23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="M71">
-        <f>(1/$B$2-1)*M35-M23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="N71">
-        <f>(1/$B$2-1)*N35-N23</f>
+        <f t="shared" si="92"/>
         <v>0</v>
       </c>
       <c r="O71">
-        <f>(1/$B$2-1)*O35-O23</f>
+        <f t="shared" si="92"/>
         <v>-1</v>
       </c>
       <c r="Q71">
-        <f>(1/$B$2-1)*Q35-Q23</f>
+        <f t="shared" ref="Q71:Z71" si="93">(1/$B$2-1)*Q35-Q23</f>
         <v>0</v>
       </c>
       <c r="R71">
-        <f>(1/$B$2-1)*R35-R23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="S71">
-        <f>(1/$B$2-1)*S35-S23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="T71">
-        <f>(1/$B$2-1)*T35-T23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="U71">
-        <f>(1/$B$2-1)*U35-U23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="V71">
-        <f>(1/$B$2-1)*V35-V23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="W71">
-        <f>(1/$B$2-1)*W35-W23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="X71">
-        <f>(1/$B$2-1)*X35-X23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="Y71">
-        <f>(1/$B$2-1)*Y35-Y23</f>
+        <f t="shared" si="93"/>
         <v>0</v>
       </c>
       <c r="Z71">
-        <f>(1/$B$2-1)*Z35-Z23</f>
+        <f t="shared" si="93"/>
         <v>-1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1">
+        <f>B2*COS(B3)</f>
+        <v>1.8406227634233914</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2">
+        <f>B2*SIN(B3)</f>
+        <v>-4.6488824294412563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <f>PI() * 1.62</f>
+        <v>5.0893800988154654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <f>SQRT(B1^2+E1^2)</f>
+        <v>10.167983681990858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <f>SQRT(B1^2+E2^2)</f>
+        <v>11.027787985029802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>E5+E1</f>
+        <v>12.868410748453194</v>
+      </c>
+      <c r="F8">
+        <f>ROUND(E8, 1)</f>
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f>E4+E2</f>
+        <v>5.5191012525496017</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F11" si="0">ROUND(E9, 1)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <f>E5-E1</f>
+        <v>9.1871652216064099</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f>E4-E2</f>
+        <v>14.816866111432114</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f>SIN(D14)</f>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="D14">
+        <f>PI()/4</f>
+        <v>0.78539816339744828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tests for MakeRHS functions
</commit_message>
<xml_diff>
--- a/unittests calculations.xlsx
+++ b/unittests calculations.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="scheme 2 LHS calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Quarter coordinates calculation" sheetId="2" r:id="rId2"/>
+    <sheet name="scheme 2 RHS calculations" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>nr</t>
   </si>
@@ -101,6 +102,75 @@
   <si>
     <t>rounded</t>
   </si>
+  <si>
+    <t>lambda_core</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>compartment</t>
+  </si>
+  <si>
+    <t>rbc core</t>
+  </si>
+  <si>
+    <t>cfl</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>vw</t>
+  </si>
+  <si>
+    <t>tissue</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>R_NO</t>
+  </si>
+  <si>
+    <t>lambda_vw</t>
+  </si>
+  <si>
+    <t>lambda_t</t>
+  </si>
+  <si>
+    <t>no.R_max</t>
+  </si>
+  <si>
+    <t>wss</t>
+  </si>
+  <si>
+    <t>wss_ref</t>
+  </si>
+  <si>
+    <t>no.q_ref</t>
+  </si>
+  <si>
+    <t>o2.Km_eNOS</t>
+  </si>
+  <si>
+    <t>r_coeff</t>
+  </si>
+  <si>
+    <t>o2.Q_max_vw</t>
+  </si>
+  <si>
+    <t>o2.Q_max_t</t>
+  </si>
+  <si>
+    <t>no.C_ref</t>
+  </si>
+  <si>
+    <t>Km</t>
+  </si>
 </sst>
 </file>
 
@@ -135,8 +205,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4880,7 +4953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -5023,4 +5096,516 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1">
+        <v>1.4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2">
+        <v>1.3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <f>$B$1*F2*$B$2</f>
+        <v>2.0020000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1.2</v>
+      </c>
+      <c r="G3">
+        <v>2.9</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H5" si="0">$B$1*F3*$B$2</f>
+        <v>2.1840000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1.3</v>
+      </c>
+      <c r="G4">
+        <v>2.8</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.3659999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1.4</v>
+      </c>
+      <c r="G5">
+        <v>2.7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>2.5479999999999996</v>
+      </c>
+      <c r="I5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>2.4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1.5</v>
+      </c>
+      <c r="G6">
+        <v>2.6</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1.6</v>
+      </c>
+      <c r="G7">
+        <v>2.5</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>1.7</v>
+      </c>
+      <c r="G8">
+        <v>2.4</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <f>B5/B6*B7</f>
+        <v>31.25</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>1.8</v>
+      </c>
+      <c r="G9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10">
+        <f>0.027</f>
+        <v>2.7E-2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>1.9</v>
+      </c>
+      <c r="G10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H10">
+        <f>-$B$9*G10/(G10+$B$11)*$B$2</f>
+        <v>-12.952898550724639</v>
+      </c>
+      <c r="I10">
+        <f>$B$2*$B$9*G10/(G10+$B$11)</f>
+        <v>12.952898550724639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>4.7</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>2.1</v>
+      </c>
+      <c r="H11">
+        <f>-$B$9*G11/(G11+$B$11)*$B$2</f>
+        <v>-12.545955882352942</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I13" si="1">$B$2*$B$9*G11/(G11+$B$11)</f>
+        <v>12.54595588235294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12">
+        <v>2.1</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <f>-$B$9*G12/(G12+$B$11)*$B$2</f>
+        <v>-12.126865671641792</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>12.126865671641792</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G13">
+        <v>1.9</v>
+      </c>
+      <c r="H13">
+        <f>-$B$9*G13/(G13+$B$11)*$B$2</f>
+        <v>-11.695075757575758</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>11.695075757575758</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G14">
+        <v>1.8</v>
+      </c>
+      <c r="H14">
+        <f>F14*$B$2</f>
+        <v>2.9899999999999998</v>
+      </c>
+      <c r="I14">
+        <f>$B$2*$B$12*G14/(G14+$B$8*(1+F14/$B$10))</f>
+        <v>0.13297693214345851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D15" s="1"/>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15">
+        <v>2.4</v>
+      </c>
+      <c r="G15">
+        <v>1.7</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H17" si="2">F15*$B$2</f>
+        <v>3.12</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I21" si="3">$B$2*$B$12*G15/(G15+$B$8*(1+F15/$B$10))</f>
+        <v>0.12064782239475917</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D16" s="1"/>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16">
+        <v>1.6</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>3.25</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>0.10925219827250798</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="1"/>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17">
+        <v>2.6</v>
+      </c>
+      <c r="G17">
+        <v>1.5</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>3.3800000000000003</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>9.8687910028116207E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>2.7</v>
+      </c>
+      <c r="G18">
+        <v>1.4</v>
+      </c>
+      <c r="H18">
+        <f>$B$4*F18*$B$2</f>
+        <v>3.5100000000000002</v>
+      </c>
+      <c r="I18">
+        <f>$B$2*$B$13*G18/(G18+$B$8*(1+F18/$B$10))</f>
+        <v>0.88867187499999978</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19">
+        <v>2.8</v>
+      </c>
+      <c r="G19">
+        <v>1.3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ref="H19:H21" si="4">$B$4*F19*$B$2</f>
+        <v>3.6399999999999997</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ref="I19:I21" si="5">$B$2*$B$13*G19/(G19+$B$8*(1+F19/$B$10))</f>
+        <v>0.79714195870165272</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20">
+        <v>19</v>
+      </c>
+      <c r="F20">
+        <v>2.9</v>
+      </c>
+      <c r="G20">
+        <v>1.2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="4"/>
+        <v>3.77</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>0.71163073595999193</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="4"/>
+        <v>3.9000000000000004</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="5"/>
+        <v>0.63156345078025322</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected quarter coordinates for circle, overloaded GetQuarterCoordinates to add quarter coordinates for ellipse, added tests for GetQuarterCoordinates for ellipse
</commit_message>
<xml_diff>
--- a/unittests calculations.xlsx
+++ b/unittests calculations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repos\gas-diffusion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LYer\Git Repos\gas-diffusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="scheme 2 LHS calculations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>nr</t>
   </si>
@@ -82,18 +82,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>x_offset</t>
-  </si>
-  <si>
-    <t>y_offset</t>
-  </si>
-  <si>
-    <t>x_dist</t>
-  </si>
-  <si>
-    <t>y_dist</t>
-  </si>
-  <si>
     <t>coordinates</t>
   </si>
   <si>
@@ -170,6 +158,57 @@
   </si>
   <si>
     <t>Km</t>
+  </si>
+  <si>
+    <t>r_front</t>
+  </si>
+  <si>
+    <t>r_back</t>
+  </si>
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>r_front + r_back</t>
+  </si>
+  <si>
+    <t>r_front - r_back</t>
+  </si>
+  <si>
+    <t>plus rounded</t>
+  </si>
+  <si>
+    <t>minus rounded</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Ellipse</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>theta0</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>sqr_sum</t>
+  </si>
+  <si>
+    <t>sqr_diff</t>
+  </si>
+  <si>
+    <t>pi_coeff</t>
   </si>
 </sst>
 </file>
@@ -4951,145 +4990,408 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E1">
-        <f>B2*COS(B3)</f>
-        <v>1.8406227634233914</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>$B$3*COS(E3-$B$4)</f>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <f>SQRT($B$2^2-$B$3^2*SIN(E3-$B$4)^2)</f>
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <f>F3+G3</f>
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <f>F3-G3</f>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f>ROUND(H3, 1)</f>
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <f>ROUND(I3, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F4">
+        <f>$B$3*COS(E4-$B$4)</f>
+        <v>6.1257422745431001E-16</v>
+      </c>
+      <c r="G4">
+        <f>SQRT($B$2^2-$B$3^2*SIN(E4-$B$4)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="0">F4+G4</f>
+        <v>6.1257422745431001E-16</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I6" si="1">F4-G4</f>
+        <v>6.1257422745431001E-16</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J6" si="2">ROUND(H4, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K6" si="3">ROUND(I4, 1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F5">
+        <f>$B$3*COS(E5-$B$4)</f>
+        <v>-10</v>
+      </c>
+      <c r="G5">
+        <f>SQRT($B$2^2-$B$3^2*SIN(E5-$B$4)^2)</f>
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>-20</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <f>1.5*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="F6">
+        <f>$B$3*COS(E6-$B$4)</f>
+        <v>-1.83772268236293E-15</v>
+      </c>
+      <c r="G6">
+        <f>SQRT($B$2^2-$B$3^2*SIN(E6-$B$4)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>-1.83772268236293E-15</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-1.83772268236293E-15</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f>$B$13*($B$12*COS(E10+$B$14-2*$B$16)+$B$11*COS(E10-$B$14))</f>
+        <v>132.52483896648417</v>
+      </c>
+      <c r="G10">
+        <f>SQRT(2)*$B$9*$B$10*SQRT(H10-2*$B$13^2*SIN(E10-$B$14)^2)</f>
+        <v>596.38683948044479</v>
+      </c>
+      <c r="H10">
+        <f>$B$12*COS(2*E10-2*$B$16)+$B$11</f>
+        <v>120.41112156779951</v>
+      </c>
+      <c r="I10">
+        <f>(F10+G10)/H10</f>
+        <v>6.0535245329186882</v>
+      </c>
+      <c r="J10">
+        <f>ROUND(I10, 1)</f>
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <f>B9^2+B10^2</f>
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <f>PI()/2</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F13" si="4">$B$13*($B$12*COS(E11+$B$14-2*$B$16)+$B$11*COS(E11-$B$14))</f>
+        <v>-334.71953491977041</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G13" si="5">SQRT(2)*$B$9*$B$10*SQRT(H11-2*$B$13^2*SIN(E11-$B$14)^2)</f>
+        <v>579.24324570470947</v>
+      </c>
+      <c r="H11">
+        <f>$B$12*COS(2*E11-2*$B$16)+$B$11</f>
+        <v>79.588878432200488</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I13" si="6">(F11+G11)/H11</f>
+        <v>3.0723351754886443</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J13" si="7">ROUND(I11, 1)</f>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12">
+        <f>B10^2-B9^2</f>
+        <v>-28</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <f>PI()</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>-132.52483896648411</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>596.38683948044479</v>
+      </c>
+      <c r="H12">
+        <f>$B$12*COS(2*E12-2*$B$16)+$B$11</f>
+        <v>120.41112156779951</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="6"/>
+        <v>3.8523185771737483</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="7"/>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <f>B2*SIN(B3)</f>
-        <v>-4.6488824294412563</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f>1.5*PI()</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>334.71953491977041</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>579.24324570470947</v>
+      </c>
+      <c r="H13">
+        <f>$B$12*COS(2*E13-2*$B$16)+$B$11</f>
+        <v>79.588878432200502</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
+        <v>11.483548940861866</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="7"/>
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <f>B15*PI()</f>
+        <v>5.0893800988154654</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
-        <f>PI() * 1.62</f>
+      <c r="B16">
+        <f>PI()*B17</f>
         <v>5.0893800988154654</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4">
-        <f>SQRT(B1^2+E1^2)</f>
-        <v>10.167983681990858</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5">
-        <f>SQRT(B1^2+E2^2)</f>
-        <v>11.027787985029802</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <f>E5+E1</f>
-        <v>12.868410748453194</v>
-      </c>
-      <c r="F8">
-        <f>ROUND(E8, 1)</f>
-        <v>12.9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
-        <f>E4+E2</f>
-        <v>5.5191012525496017</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ref="F9:F11" si="0">ROUND(E9, 1)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <f>E5-E1</f>
-        <v>9.1871652216064099</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <f>E4-E2</f>
-        <v>14.816866111432114</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>14.8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <f>SIN(D14)</f>
-        <v>0.70710678118654746</v>
-      </c>
-      <c r="D14">
-        <f>PI()/4</f>
-        <v>0.78539816339744828</v>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17">
+        <v>1.62</v>
       </c>
     </row>
   </sheetData>
@@ -5102,7 +5404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10:I20"/>
     </sheetView>
   </sheetViews>
@@ -5114,36 +5416,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1">
         <v>1.4</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>1.3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -5161,7 +5463,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5183,7 +5485,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5205,7 +5507,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>1.5</v>
@@ -5230,13 +5532,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>2.4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -5256,7 +5558,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B7">
         <v>50</v>
@@ -5280,7 +5582,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5304,7 +5606,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <f>B5/B6*B7</f>
@@ -5329,14 +5631,14 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <f>0.027</f>
         <v>2.7E-2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>9</v>
@@ -5358,7 +5660,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>4.7</v>
@@ -5384,7 +5686,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -5410,7 +5712,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -5436,7 +5738,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E14">
         <v>13</v>
@@ -5472,7 +5774,7 @@
         <v>3.12</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="I15:I21" si="3">$B$2*$B$12*G15/(G15+$B$8*(1+F15/$B$10))</f>
+        <f t="shared" ref="I15:I17" si="3">$B$2*$B$12*G15/(G15+$B$8*(1+F15/$B$10))</f>
         <v>0.12064782239475917</v>
       </c>
     </row>
@@ -5518,7 +5820,7 @@
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E18">
         <v>17</v>

</xml_diff>

<commit_message>
implemented WSS calculation based on CFL width and edge velocity
</commit_message>
<xml_diff>
--- a/unittests calculations.xlsx
+++ b/unittests calculations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LYer\Git Repos\gas-diffusion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repos\gas-diffusion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="scheme 2 LHS calculations" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>nr</t>
   </si>
@@ -209,6 +209,12 @@
   </si>
   <si>
     <t>pi_coeff</t>
+  </si>
+  <si>
+    <t>edge_vel</t>
+  </si>
+  <si>
+    <t>viscosity</t>
   </si>
 </sst>
 </file>
@@ -4992,7 +4998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
@@ -5404,8 +5410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5510,7 +5516,8 @@
         <v>35</v>
       </c>
       <c r="B5">
-        <v>1.5</v>
+        <f>B16*B15/B17</f>
+        <v>0.30232558139534887</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5">
@@ -5610,7 +5617,7 @@
       </c>
       <c r="B9">
         <f>B5/B6*B7</f>
-        <v>31.25</v>
+        <v>6.2984496124031022</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9">
@@ -5651,11 +5658,11 @@
       </c>
       <c r="H10">
         <f>-$B$9*G10/(G10+$B$11)*$B$2</f>
-        <v>-12.952898550724639</v>
+        <v>-2.6106617234018659</v>
       </c>
       <c r="I10">
         <f>$B$2*$B$9*G10/(G10+$B$11)</f>
-        <v>12.952898550724639</v>
+        <v>2.6106617234018654</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5677,11 +5684,11 @@
       </c>
       <c r="H11">
         <f>-$B$9*G11/(G11+$B$11)*$B$2</f>
-        <v>-12.545955882352942</v>
+        <v>-2.5286422708618339</v>
       </c>
       <c r="I11">
         <f t="shared" ref="I11:I13" si="1">$B$2*$B$9*G11/(G11+$B$11)</f>
-        <v>12.54595588235294</v>
+        <v>2.5286422708618335</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -5703,11 +5710,11 @@
       </c>
       <c r="H12">
         <f>-$B$9*G12/(G12+$B$11)*$B$2</f>
-        <v>-12.126865671641792</v>
+        <v>-2.4441744764549354</v>
       </c>
       <c r="I12">
         <f t="shared" si="1"/>
-        <v>12.126865671641792</v>
+        <v>2.4441744764549349</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -5729,11 +5736,11 @@
       </c>
       <c r="H13">
         <f>-$B$9*G13/(G13+$B$11)*$B$2</f>
-        <v>-11.695075757575758</v>
+        <v>-2.3571470519144944</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>11.695075757575758</v>
+        <v>2.3571470519144944</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -5759,6 +5766,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15">
         <v>14</v>
@@ -5779,6 +5792,12 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16">
+        <v>1.3</v>
+      </c>
       <c r="D16" s="1"/>
       <c r="E16">
         <v>15</v>
@@ -5798,7 +5817,13 @@
         <v>0.10925219827250798</v>
       </c>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17">
+        <v>4.3</v>
+      </c>
       <c r="D17" s="1"/>
       <c r="E17">
         <v>16</v>
@@ -5818,7 +5843,7 @@
         <v>9.8687910028116207E-2</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
         <v>28</v>
       </c>
@@ -5840,7 +5865,7 @@
         <v>0.88867187499999978</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19">
         <v>18</v>
@@ -5860,7 +5885,7 @@
         <v>0.79714195870165272</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20">
         <v>19</v>
@@ -5880,7 +5905,7 @@
         <v>0.71163073595999193</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D21" s="1"/>
       <c r="E21">
         <v>20</v>
@@ -5909,5 +5934,6 @@
     <mergeCell ref="D18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>